<commit_message>
link and script tags corrected
</commit_message>
<xml_diff>
--- a/account-data.xlsx
+++ b/account-data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -445,17 +445,31 @@
         <v>bee</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>bibi</v>
+      </c>
+      <c r="C4" t="str">
+        <v>123</v>
+      </c>
+      <c r="D4" t="str">
+        <v>bear</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -526,9 +540,20 @@
         <v xml:space="preserve">Gilbert Keith Chesterton </v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>3</v>
+      </c>
+      <c r="B7" t="str">
+        <v>In Cold Blood</v>
+      </c>
+      <c r="C7" t="str">
+        <v xml:space="preserve">Truman Capote </v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>